<commit_message>
dragon fujimi and t&t
</commit_message>
<xml_diff>
--- a/tunnels-trolls-kadokawa/checklist.xlsx
+++ b/tunnels-trolls-kadokawa/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tunnels-trolls-kadokawa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB81A765-0496-CB48-BD5A-94D24A44DAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F66AB6-877B-AB4D-A0D7-B23AD20DCC17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{ADE42680-67A1-2B4B-9DF7-DE4808BB346E}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>ドラゴン大陸 ハイパーT＆Tワールドガイド</t>
   </si>
   <si>
-    <t>Dragon Contient: Hyper T&amp;T World Guide</t>
-  </si>
-  <si>
     <t>dragon_continent.jpg</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>drops_from_the_sky.jpg</t>
+  </si>
+  <si>
+    <t>Dragon Continent: Hyper T&amp;T World Guide</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,16 +534,16 @@
         <v>1994</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -551,16 +551,16 @@
         <v>1994</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -568,16 +568,16 @@
         <v>1994</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -605,13 +605,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -619,16 +619,16 @@
         <v>1996</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
product_type for t&t kadokawa
</commit_message>
<xml_diff>
--- a/tunnels-trolls-kadokawa/checklist.xlsx
+++ b/tunnels-trolls-kadokawa/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/tunnels-trolls-kadokawa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F66AB6-877B-AB4D-A0D7-B23AD20DCC17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0D0A2-D83D-BC40-9106-100DA04D38C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{ADE42680-67A1-2B4B-9DF7-DE4808BB346E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{ADE42680-67A1-2B4B-9DF7-DE4808BB346E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>year</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Dragon Continent: Hyper T&amp;T World Guide</t>
+  </si>
+  <si>
+    <t>product_type</t>
+  </si>
+  <si>
+    <t>rulebook</t>
+  </si>
+  <si>
+    <t>replay</t>
+  </si>
+  <si>
+    <t>supplement</t>
   </si>
 </sst>
 </file>
@@ -482,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F22FC8A-0C0B-AE48-A487-D3FEA4C8A745}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +507,7 @@
     <col min="5" max="5" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +523,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1994</v>
       </c>
@@ -528,8 +543,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1994</v>
       </c>
@@ -545,8 +563,11 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1994</v>
       </c>
@@ -562,8 +583,11 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1994</v>
       </c>
@@ -579,8 +603,11 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1995</v>
       </c>
@@ -596,8 +623,11 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1995</v>
       </c>
@@ -613,8 +643,11 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1996</v>
       </c>
@@ -629,6 +662,9 @@
       </c>
       <c r="E8" t="s">
         <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>